<commit_message>
WindowWelcome.pyw rewriting Start.pyw - small fixes
</commit_message>
<xml_diff>
--- a/2021-2022.xlsx
+++ b/2021-2022.xlsx
@@ -170,7 +170,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="10"/>
       <name val="Arial Cyr"/>
@@ -327,6 +327,11 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="20"/>
       <name val="Neucha"/>
       <family val="3"/>
@@ -391,7 +396,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC0C0C0"/>
-        <bgColor rgb="FFDDD9C3"/>
+        <bgColor rgb="FFB3B3B3"/>
       </patternFill>
     </fill>
     <fill>
@@ -615,23 +620,23 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="5" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -639,51 +644,51 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="22" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="5" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="23" fillId="5" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -691,15 +696,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="25" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -750,7 +755,7 @@
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFB3B3B3"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFDDD9C3"/>
@@ -835,15 +840,15 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0771862117358126"/>
-          <c:y val="0.0308143219264892"/>
-          <c:w val="0.88470309621963"/>
-          <c:h val="0.875"/>
+          <c:x val="0.0772217617032416"/>
+          <c:y val="0.030824088748019"/>
+          <c:w val="0.884516382356791"/>
+          <c:h val="0.874643423137876"/>
         </c:manualLayout>
       </c:layout>
       <c:bar3DChart>
         <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+        <c:grouping val="standard"/>
         <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
@@ -1565,13 +1570,13 @@
                   <c:v>42000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>32000</c:v>
+                  <c:v>36000</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>12000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>43000</c:v>
+                  <c:v>47000</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>34000</c:v>
@@ -1594,12 +1599,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="cylinder"/>
-        <c:axId val="48909965"/>
-        <c:axId val="33933980"/>
-        <c:axId val="0"/>
+        <c:axId val="43698573"/>
+        <c:axId val="60250227"/>
+        <c:axId val="34504902"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="48909965"/>
+        <c:axId val="43698573"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1642,7 +1647,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="33933980"/>
+        <c:crossAx val="60250227"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1650,7 +1655,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="33933980"/>
+        <c:axId val="60250227"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1693,13 +1698,45 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="48909965"/>
+        <c:crossAx val="43698573"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:serAx>
+        <c:axId val="34504902"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln w="0">
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="60250227"/>
+        <c:crosses val="autoZero"/>
+      </c:serAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
+    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1728,10 +1765,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.118550761746255"/>
-          <c:y val="0.0636177347242921"/>
-          <c:w val="0.840225323262066"/>
-          <c:h val="0.747298807749627"/>
+          <c:x val="0.118468009176651"/>
+          <c:y val="0.0636414461423779"/>
+          <c:w val="0.840045883252613"/>
+          <c:h val="0.747204621692136"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1846,7 +1883,7 @@
                   <c:v>66000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>98000</c:v>
+                  <c:v>106000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1861,11 +1898,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="14594464"/>
-        <c:axId val="61459192"/>
+        <c:axId val="22860531"/>
+        <c:axId val="51173780"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="14594464"/>
+        <c:axId val="22860531"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1907,7 +1944,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61459192"/>
+        <c:crossAx val="51173780"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1915,7 +1952,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61459192"/>
+        <c:axId val="51173780"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1957,7 +1994,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="14594464"/>
+        <c:crossAx val="22860531"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1996,9 +2033,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>609840</xdr:colOff>
+      <xdr:colOff>608400</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>164160</xdr:rowOff>
+      <xdr:rowOff>162720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2006,8 +2043,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4784040" y="38160"/>
-        <a:ext cx="8208360" cy="4544280"/>
+        <a:off x="4867200" y="38160"/>
+        <a:ext cx="8251200" cy="4542840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2031,9 +2068,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>551880</xdr:colOff>
+      <xdr:colOff>550440</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>73800</xdr:rowOff>
+      <xdr:rowOff>72360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2041,8 +2078,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4906080" y="0"/>
-        <a:ext cx="5623560" cy="3864600"/>
+        <a:off x="4910400" y="0"/>
+        <a:ext cx="5648760" cy="3863160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2063,12 +2100,12 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="3.33"/>
@@ -2269,13 +2306,13 @@
         <v>1000</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E10" s="8"/>
       <c r="F10" s="9"/>
       <c r="G10" s="7" t="n">
         <f aca="false">C10*(D10-E10)</f>
-        <v>32000</v>
+        <v>36000</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2309,13 +2346,13 @@
         <v>1000</v>
       </c>
       <c r="D12" s="6" t="n">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="9"/>
       <c r="G12" s="7" t="n">
         <f aca="false">C12*(D12-E12)</f>
-        <v>43000</v>
+        <v>47000</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2451,7 +2488,7 @@
       <c r="C20" s="7"/>
       <c r="D20" s="20" t="n">
         <f aca="false">SUM(D2:D19)</f>
-        <v>643</v>
+        <v>651</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="21" t="n">
@@ -2460,7 +2497,7 @@
       </c>
       <c r="G20" s="20" t="n">
         <f aca="false">SUM(G2:G19)</f>
-        <v>643500</v>
+        <v>651500</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2474,7 +2511,7 @@
       <c r="F21" s="23"/>
       <c r="G21" s="24" t="n">
         <f aca="false">F20+G20</f>
-        <v>643500</v>
+        <v>651500</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2509,7 +2546,7 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83984375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.44"/>
@@ -2750,19 +2787,19 @@
       </c>
       <c r="B10" s="44" t="n">
         <f aca="false">Приходы!$D$20</f>
-        <v>643</v>
+        <v>651</v>
       </c>
       <c r="C10" s="43" t="n">
         <f aca="false">Приходы!$G$20</f>
-        <v>643500</v>
+        <v>651500</v>
       </c>
       <c r="D10" s="45" t="n">
         <f aca="false">B10-B9</f>
-        <v>97.5</v>
+        <v>105.5</v>
       </c>
       <c r="E10" s="46" t="n">
         <f aca="false">C10-C9</f>
-        <v>98000</v>
+        <v>106000</v>
       </c>
       <c r="F10" s="43" t="n">
         <f aca="false">ROUND(E10/D10,0)</f>

</xml_diff>

<commit_message>
Minor corrections and adds
</commit_message>
<xml_diff>
--- a/2021-2022.xlsx
+++ b/2021-2022.xlsx
@@ -840,10 +840,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0772217617032416"/>
-          <c:y val="0.030824088748019"/>
-          <c:w val="0.884516382356791"/>
-          <c:h val="0.874643423137876"/>
+          <c:x val="0.0772509786863854"/>
+          <c:y val="0.0308289744809003"/>
+          <c:w val="0.884428012179208"/>
+          <c:h val="0.874465049928673"/>
         </c:manualLayout>
       </c:layout>
       <c:bar3DChart>
@@ -1576,7 +1576,7 @@
                   <c:v>12000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>47000</c:v>
+                  <c:v>49000</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>34000</c:v>
@@ -1599,12 +1599,12 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:shape val="cylinder"/>
-        <c:axId val="43698573"/>
-        <c:axId val="60250227"/>
-        <c:axId val="34504902"/>
+        <c:axId val="74747794"/>
+        <c:axId val="67442132"/>
+        <c:axId val="1442545"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="43698573"/>
+        <c:axId val="74747794"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1647,7 +1647,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60250227"/>
+        <c:crossAx val="67442132"/>
         <c:crossesAt val="0"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1655,7 +1655,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60250227"/>
+        <c:axId val="67442132"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1698,12 +1698,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43698573"/>
+        <c:crossAx val="74747794"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:serAx>
-        <c:axId val="34504902"/>
+        <c:axId val="1442545"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1731,7 +1731,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60250227"/>
+        <c:crossAx val="67442132"/>
         <c:crosses val="autoZero"/>
       </c:serAx>
     </c:plotArea>
@@ -1765,10 +1765,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.118468009176651"/>
-          <c:y val="0.0636414461423779"/>
-          <c:w val="0.840045883252613"/>
-          <c:h val="0.747204621692136"/>
+          <c:x val="0.11841352571029"/>
+          <c:y val="0.0636533084808947"/>
+          <c:w val="0.839954236318566"/>
+          <c:h val="0.747157502329916"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1883,7 +1883,7 @@
                   <c:v>66000</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>106000</c:v>
+                  <c:v>108000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1898,11 +1898,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="22860531"/>
-        <c:axId val="51173780"/>
+        <c:axId val="77902220"/>
+        <c:axId val="8676863"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="22860531"/>
+        <c:axId val="77902220"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1944,7 +1944,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51173780"/>
+        <c:crossAx val="8676863"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1952,7 +1952,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51173780"/>
+        <c:axId val="8676863"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1994,7 +1994,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22860531"/>
+        <c:crossAx val="77902220"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2033,9 +2033,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>608400</xdr:colOff>
+      <xdr:colOff>607680</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>162720</xdr:rowOff>
+      <xdr:rowOff>162000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2043,8 +2043,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4867200" y="38160"/>
-        <a:ext cx="8251200" cy="4542840"/>
+        <a:off x="4872240" y="38160"/>
+        <a:ext cx="8276040" cy="4542120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2068,9 +2068,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>550440</xdr:colOff>
+      <xdr:colOff>549720</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>72360</xdr:rowOff>
+      <xdr:rowOff>71640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2078,8 +2078,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4910400" y="0"/>
-        <a:ext cx="5648760" cy="3863160"/>
+        <a:off x="4912920" y="0"/>
+        <a:ext cx="5663520" cy="3862440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2100,10 +2100,10 @@
   <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.94140625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.81"/>
@@ -2306,9 +2306,11 @@
         <v>1000</v>
       </c>
       <c r="D10" s="6" t="n">
-        <v>36</v>
-      </c>
-      <c r="E10" s="8"/>
+        <v>38</v>
+      </c>
+      <c r="E10" s="8" t="n">
+        <v>2</v>
+      </c>
       <c r="F10" s="9"/>
       <c r="G10" s="7" t="n">
         <f aca="false">C10*(D10-E10)</f>
@@ -2346,13 +2348,13 @@
         <v>1000</v>
       </c>
       <c r="D12" s="6" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E12" s="8"/>
       <c r="F12" s="9"/>
       <c r="G12" s="7" t="n">
         <f aca="false">C12*(D12-E12)</f>
-        <v>47000</v>
+        <v>49000</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2488,7 +2490,7 @@
       <c r="C20" s="7"/>
       <c r="D20" s="20" t="n">
         <f aca="false">SUM(D2:D19)</f>
-        <v>651</v>
+        <v>655</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="21" t="n">
@@ -2497,7 +2499,7 @@
       </c>
       <c r="G20" s="20" t="n">
         <f aca="false">SUM(G2:G19)</f>
-        <v>651500</v>
+        <v>653500</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2511,7 +2513,7 @@
       <c r="F21" s="23"/>
       <c r="G21" s="24" t="n">
         <f aca="false">F20+G20</f>
-        <v>651500</v>
+        <v>653500</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2546,7 +2548,7 @@
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.94140625" defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.44"/>
@@ -2787,23 +2789,23 @@
       </c>
       <c r="B10" s="44" t="n">
         <f aca="false">Приходы!$D$20</f>
-        <v>651</v>
+        <v>655</v>
       </c>
       <c r="C10" s="43" t="n">
         <f aca="false">Приходы!$G$20</f>
-        <v>651500</v>
+        <v>653500</v>
       </c>
       <c r="D10" s="45" t="n">
         <f aca="false">B10-B9</f>
-        <v>105.5</v>
+        <v>109.5</v>
       </c>
       <c r="E10" s="46" t="n">
         <f aca="false">C10-C9</f>
-        <v>106000</v>
+        <v>108000</v>
       </c>
       <c r="F10" s="43" t="n">
         <f aca="false">ROUND(E10/D10,0)</f>
-        <v>1005</v>
+        <v>986</v>
       </c>
       <c r="I10" s="35"/>
     </row>

</xml_diff>